<commit_message>
proper simulation for one team
</commit_message>
<xml_diff>
--- a/schedules.xlsx
+++ b/schedules.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89D3B78-75AF-4E7E-BB81-A5DE3A1EC65A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83443365-84C5-460F-95ED-3F5DBF970FC3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="14-15" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="62">
   <si>
     <t>Team</t>
   </si>
@@ -48,13 +48,7 @@
     <t>BOS</t>
   </si>
   <si>
-    <t>BRK</t>
-  </si>
-  <si>
     <t>CHI</t>
-  </si>
-  <si>
-    <t>CHO</t>
   </si>
   <si>
     <t>CLE</t>
@@ -96,9 +90,6 @@
     <t>MIN</t>
   </si>
   <si>
-    <t>NOP</t>
-  </si>
-  <si>
     <t>NYK</t>
   </si>
   <si>
@@ -138,13 +129,7 @@
     <t>Boston Celtics</t>
   </si>
   <si>
-    <t>Brooklyn Nets</t>
-  </si>
-  <si>
     <t>Chicago Bulls</t>
-  </si>
-  <si>
-    <t>Charlotte Hornets</t>
   </si>
   <si>
     <t>Cleveland Cavaliers</t>
@@ -184,9 +169,6 @@
   </si>
   <si>
     <t>Minnesota Timberwolves</t>
-  </si>
-  <si>
-    <t>New Orleans Pelicans</t>
   </si>
   <si>
     <t>New York Knicks</t>
@@ -238,6 +220,9 @@
   </si>
   <si>
     <t>New Orleans Hornets</t>
+  </si>
+  <si>
+    <t>SEA</t>
   </si>
 </sst>
 </file>
@@ -557,11 +542,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -574,93 +562,93 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
+        <v>61</v>
+      </c>
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>27</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -755,7 +743,7 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -850,7 +838,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -945,7 +933,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1040,7 +1028,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -1135,7 +1123,7 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -1230,7 +1218,7 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1325,7 +1313,7 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -1420,7 +1408,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -1515,7 +1503,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -1610,7 +1598,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -1705,7 +1693,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -1800,7 +1788,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -1895,7 +1883,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -1990,7 +1978,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -2085,7 +2073,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -2180,7 +2168,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -2275,7 +2263,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -2370,7 +2358,7 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -2465,7 +2453,7 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -2560,7 +2548,7 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -2655,7 +2643,7 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="B23">
         <v>4</v>
@@ -2750,7 +2738,7 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -2845,7 +2833,7 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -2940,7 +2928,7 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -3035,7 +3023,7 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -3130,7 +3118,7 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -3225,7 +3213,7 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="B29">
         <v>4</v>
@@ -3320,7 +3308,7 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -3415,7 +3403,7 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B31">
         <v>4</v>
@@ -3518,7 +3506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A6F107-4E97-477D-AA04-F5D4B5E4610F}">
   <dimension ref="A1:AE31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -3538,93 +3526,93 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" t="s">
-        <v>62</v>
-      </c>
-      <c r="T1" t="s">
-        <v>63</v>
-      </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>27</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3719,7 +3707,7 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -3814,7 +3802,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -3909,7 +3897,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -4004,7 +3992,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -4099,7 +4087,7 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -4194,7 +4182,7 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -4289,7 +4277,7 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -4384,7 +4372,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -4479,7 +4467,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -4574,7 +4562,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -4669,7 +4657,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -4764,7 +4752,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -4859,7 +4847,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -4954,7 +4942,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -5049,7 +5037,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -5144,7 +5132,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -5239,7 +5227,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -5334,7 +5322,7 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -5429,7 +5417,7 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -5524,7 +5512,7 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -5619,7 +5607,7 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B23">
         <v>4</v>
@@ -5714,7 +5702,7 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -5809,7 +5797,7 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -5904,7 +5892,7 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -5999,7 +5987,7 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -6094,7 +6082,7 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -6189,7 +6177,7 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B29">
         <v>4</v>
@@ -6284,7 +6272,7 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -6379,7 +6367,7 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B31">
         <v>4</v>

</xml_diff>

<commit_message>
fixing data and programs
</commit_message>
<xml_diff>
--- a/schedules.xlsx
+++ b/schedules.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83443365-84C5-460F-95ED-3F5DBF970FC3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DDED76-C0E2-4AA5-936A-52C00A81E7EF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -542,8 +542,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,52 +563,52 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
         <v>56</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" t="s">
-        <v>16</v>
       </c>
       <c r="T1" t="s">
         <v>57</v>
@@ -616,25 +617,25 @@
         <v>17</v>
       </c>
       <c r="V1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" t="s">
         <v>61</v>
-      </c>
-      <c r="W1" t="s">
-        <v>19</v>
-      </c>
-      <c r="X1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>24</v>
       </c>
       <c r="AC1" t="s">
         <v>25</v>
@@ -666,25 +667,25 @@
         <v>4</v>
       </c>
       <c r="G2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H2">
         <v>2</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K2">
         <v>2</v>
       </c>
       <c r="L2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N2">
         <v>2</v>
@@ -693,16 +694,16 @@
         <v>2</v>
       </c>
       <c r="P2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q2">
         <v>4</v>
       </c>
       <c r="R2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T2">
         <v>2</v>
@@ -711,13 +712,13 @@
         <v>3</v>
       </c>
       <c r="V2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W2">
         <v>4</v>
       </c>
       <c r="X2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Y2">
         <v>2</v>
@@ -741,7 +742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -761,25 +762,25 @@
         <v>4</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K3">
         <v>2</v>
       </c>
       <c r="L3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N3">
         <v>2</v>
@@ -788,16 +789,16 @@
         <v>2</v>
       </c>
       <c r="P3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T3">
         <v>2</v>
@@ -806,13 +807,13 @@
         <v>4</v>
       </c>
       <c r="V3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W3">
         <v>4</v>
       </c>
       <c r="X3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Y3">
         <v>2</v>
@@ -838,7 +839,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -856,25 +857,25 @@
         <v>3</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H4">
         <v>2</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K4">
         <v>2</v>
       </c>
       <c r="L4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N4">
         <v>2</v>
@@ -883,16 +884,16 @@
         <v>2</v>
       </c>
       <c r="P4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T4">
         <v>2</v>
@@ -901,13 +902,13 @@
         <v>4</v>
       </c>
       <c r="V4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W4">
         <v>3</v>
       </c>
       <c r="X4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Y4">
         <v>2</v>
@@ -951,25 +952,25 @@
         <v>4</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H5">
         <v>2</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K5">
         <v>2</v>
       </c>
       <c r="L5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N5">
         <v>2</v>
@@ -978,16 +979,16 @@
         <v>2</v>
       </c>
       <c r="P5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T5">
         <v>2</v>
@@ -996,13 +997,13 @@
         <v>3</v>
       </c>
       <c r="V5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Y5">
         <v>2</v>
@@ -1028,7 +1029,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -1046,25 +1047,25 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H6">
         <v>2</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K6">
         <v>2</v>
       </c>
       <c r="L6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N6">
         <v>2</v>
@@ -1073,31 +1074,31 @@
         <v>2</v>
       </c>
       <c r="P6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q6">
         <v>4</v>
       </c>
       <c r="R6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T6">
         <v>2</v>
       </c>
       <c r="U6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Y6">
         <v>2</v>
@@ -1123,28 +1124,28 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I7">
         <v>2</v>
@@ -1153,72 +1154,72 @@
         <v>4</v>
       </c>
       <c r="K7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L7">
         <v>2</v>
       </c>
       <c r="M7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P7">
         <v>2</v>
       </c>
       <c r="Q7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S7">
         <v>2</v>
       </c>
       <c r="T7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V7">
         <v>2</v>
       </c>
       <c r="W7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Y7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Z7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AB7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AC7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AD7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AE7">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1236,43 +1237,43 @@
         <v>2</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K8">
         <v>4</v>
       </c>
       <c r="L8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q8">
         <v>2</v>
       </c>
       <c r="R8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T8">
         <v>4</v>
@@ -1281,13 +1282,13 @@
         <v>2</v>
       </c>
       <c r="V8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="W8">
         <v>2</v>
       </c>
       <c r="X8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y8">
         <v>4</v>
@@ -1296,7 +1297,7 @@
         <v>4</v>
       </c>
       <c r="AA8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB8">
         <v>4</v>
@@ -1313,28 +1314,28 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G9">
         <v>2</v>
       </c>
       <c r="H9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1343,7 +1344,7 @@
         <v>2</v>
       </c>
       <c r="K9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L9">
         <v>4</v>
@@ -1352,84 +1353,84 @@
         <v>2</v>
       </c>
       <c r="N9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P9">
         <v>3</v>
       </c>
       <c r="Q9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R9">
         <v>2</v>
       </c>
       <c r="S9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V9">
         <v>4</v>
       </c>
       <c r="W9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X9">
         <v>2</v>
       </c>
       <c r="Y9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Z9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AA9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AC9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AE9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G10">
         <v>4</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I10">
         <v>2</v>
@@ -1438,7 +1439,7 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L10">
         <v>2</v>
@@ -1447,16 +1448,16 @@
         <v>4</v>
       </c>
       <c r="N10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P10">
         <v>2</v>
       </c>
       <c r="Q10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R10">
         <v>4</v>
@@ -1465,45 +1466,45 @@
         <v>2</v>
       </c>
       <c r="T10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V10">
         <v>2</v>
       </c>
       <c r="W10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X10">
         <v>4</v>
       </c>
       <c r="Y10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Z10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AA10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AC10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AD10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AE10">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -1521,43 +1522,43 @@
         <v>2</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H11">
         <v>4</v>
       </c>
       <c r="I11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O11">
         <v>4</v>
       </c>
       <c r="P11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q11">
         <v>2</v>
       </c>
       <c r="R11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T11">
         <v>4</v>
@@ -1566,16 +1567,16 @@
         <v>2</v>
       </c>
       <c r="V11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="W11">
         <v>2</v>
       </c>
       <c r="X11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Y11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z11">
         <v>3</v>
@@ -1598,28 +1599,28 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G12">
         <v>2</v>
       </c>
       <c r="H12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I12">
         <v>4</v>
@@ -1628,7 +1629,7 @@
         <v>2</v>
       </c>
       <c r="K12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -1637,84 +1638,84 @@
         <v>2</v>
       </c>
       <c r="N12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P12">
         <v>4</v>
       </c>
       <c r="Q12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R12">
         <v>2</v>
       </c>
       <c r="S12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V12">
         <v>3</v>
       </c>
       <c r="W12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X12">
         <v>2</v>
       </c>
       <c r="Y12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Z12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AC12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AE12">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I13">
         <v>2</v>
@@ -1723,7 +1724,7 @@
         <v>4</v>
       </c>
       <c r="K13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L13">
         <v>2</v>
@@ -1732,63 +1733,63 @@
         <v>0</v>
       </c>
       <c r="N13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P13">
         <v>2</v>
       </c>
       <c r="Q13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S13">
         <v>2</v>
       </c>
       <c r="T13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V13">
         <v>2</v>
       </c>
       <c r="W13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X13">
         <v>4</v>
       </c>
       <c r="Y13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Z13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AA13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AB13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AC13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AD13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AE13">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -1806,25 +1807,25 @@
         <v>2</v>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -1833,31 +1834,31 @@
         <v>4</v>
       </c>
       <c r="P14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q14">
         <v>2</v>
       </c>
       <c r="R14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U14">
         <v>2</v>
       </c>
       <c r="V14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W14">
         <v>2</v>
       </c>
       <c r="X14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Y14">
         <v>4</v>
@@ -1866,16 +1867,16 @@
         <v>4</v>
       </c>
       <c r="AA14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC14">
         <v>2</v>
       </c>
       <c r="AD14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE14">
         <v>2</v>
@@ -1883,7 +1884,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -1901,25 +1902,25 @@
         <v>2</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K15">
         <v>4</v>
       </c>
       <c r="L15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N15">
         <v>4</v>
@@ -1928,16 +1929,16 @@
         <v>0</v>
       </c>
       <c r="P15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q15">
         <v>2</v>
       </c>
       <c r="R15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T15">
         <v>4</v>
@@ -1946,13 +1947,13 @@
         <v>2</v>
       </c>
       <c r="V15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W15">
         <v>2</v>
       </c>
       <c r="X15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y15">
         <v>4</v>
@@ -1964,13 +1965,13 @@
         <v>4</v>
       </c>
       <c r="AB15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC15">
         <v>2</v>
       </c>
       <c r="AD15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE15">
         <v>2</v>
@@ -1978,28 +1979,28 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G16">
         <v>2</v>
       </c>
       <c r="H16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I16">
         <v>3</v>
@@ -2008,7 +2009,7 @@
         <v>2</v>
       </c>
       <c r="K16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L16">
         <v>4</v>
@@ -2017,99 +2018,99 @@
         <v>2</v>
       </c>
       <c r="N16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P16">
         <v>0</v>
       </c>
       <c r="Q16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R16">
         <v>2</v>
       </c>
       <c r="S16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V16">
         <v>4</v>
       </c>
       <c r="W16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X16">
         <v>2</v>
       </c>
       <c r="Y16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Z16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AA16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AC16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AE16">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>4</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F17">
         <v>4</v>
       </c>
       <c r="G17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H17">
         <v>2</v>
       </c>
       <c r="I17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K17">
         <v>2</v>
       </c>
       <c r="L17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N17">
         <v>2</v>
@@ -2118,31 +2119,31 @@
         <v>2</v>
       </c>
       <c r="P17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q17">
         <v>0</v>
       </c>
       <c r="R17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T17">
         <v>2</v>
       </c>
       <c r="U17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W17">
         <v>4</v>
       </c>
       <c r="X17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Y17">
         <v>2</v>
@@ -2163,33 +2164,33 @@
         <v>2</v>
       </c>
       <c r="AE17">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I18">
         <v>2</v>
@@ -2198,25 +2199,25 @@
         <v>4</v>
       </c>
       <c r="K18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L18">
         <v>2</v>
       </c>
       <c r="M18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P18">
         <v>2</v>
       </c>
       <c r="Q18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R18">
         <v>0</v>
@@ -2225,93 +2226,93 @@
         <v>2</v>
       </c>
       <c r="T18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V18">
         <v>2</v>
       </c>
       <c r="W18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X18">
         <v>4</v>
       </c>
       <c r="Y18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Z18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AB18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AC18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AD18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AE18">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G19">
         <v>2</v>
       </c>
       <c r="H19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J19">
         <v>2</v>
       </c>
       <c r="K19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M19">
         <v>2</v>
       </c>
       <c r="N19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R19">
         <v>2</v>
@@ -2320,40 +2321,40 @@
         <v>0</v>
       </c>
       <c r="T19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X19">
         <v>2</v>
       </c>
       <c r="Y19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Z19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AA19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AC19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AE19">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
@@ -2376,43 +2377,43 @@
         <v>2</v>
       </c>
       <c r="G20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H20">
         <v>4</v>
       </c>
       <c r="I20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K20">
         <v>4</v>
       </c>
       <c r="L20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O20">
         <v>4</v>
       </c>
       <c r="P20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q20">
         <v>2</v>
       </c>
       <c r="R20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T20">
         <v>0</v>
@@ -2421,19 +2422,19 @@
         <v>2</v>
       </c>
       <c r="V20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="W20">
         <v>2</v>
       </c>
       <c r="X20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y20">
         <v>3</v>
       </c>
       <c r="Z20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AA20">
         <v>4</v>
@@ -2468,28 +2469,28 @@
         <v>3</v>
       </c>
       <c r="F21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H21">
         <v>2</v>
       </c>
       <c r="I21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K21">
         <v>2</v>
       </c>
       <c r="L21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N21">
         <v>2</v>
@@ -2498,16 +2499,16 @@
         <v>2</v>
       </c>
       <c r="P21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T21">
         <v>2</v>
@@ -2516,13 +2517,13 @@
         <v>0</v>
       </c>
       <c r="V21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W21">
         <v>4</v>
       </c>
       <c r="X21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Y21">
         <v>2</v>
@@ -2548,28 +2549,28 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G22">
         <v>2</v>
       </c>
       <c r="H22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I22">
         <v>4</v>
@@ -2578,7 +2579,7 @@
         <v>2</v>
       </c>
       <c r="K22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L22">
         <v>3</v>
@@ -2587,63 +2588,63 @@
         <v>2</v>
       </c>
       <c r="N22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P22">
         <v>4</v>
       </c>
       <c r="Q22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R22">
         <v>2</v>
       </c>
       <c r="S22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V22">
         <v>0</v>
       </c>
       <c r="W22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X22">
         <v>2</v>
       </c>
       <c r="Y22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Z22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AA22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AE22">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B23">
         <v>4</v>
@@ -2655,31 +2656,31 @@
         <v>3</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H23">
         <v>2</v>
       </c>
       <c r="I23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K23">
         <v>2</v>
       </c>
       <c r="L23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N23">
         <v>2</v>
@@ -2688,16 +2689,16 @@
         <v>2</v>
       </c>
       <c r="P23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q23">
         <v>4</v>
       </c>
       <c r="R23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T23">
         <v>2</v>
@@ -2706,13 +2707,13 @@
         <v>4</v>
       </c>
       <c r="V23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W23">
         <v>0</v>
       </c>
       <c r="X23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Y23">
         <v>2</v>
@@ -2738,28 +2739,28 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I24">
         <v>2</v>
@@ -2768,7 +2769,7 @@
         <v>4</v>
       </c>
       <c r="K24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L24">
         <v>2</v>
@@ -2777,16 +2778,16 @@
         <v>4</v>
       </c>
       <c r="N24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P24">
         <v>2</v>
       </c>
       <c r="Q24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R24">
         <v>4</v>
@@ -2795,45 +2796,45 @@
         <v>2</v>
       </c>
       <c r="T24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V24">
         <v>2</v>
       </c>
       <c r="W24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X24">
         <v>0</v>
       </c>
       <c r="Y24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Z24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AA24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AB24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AC24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AD24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE24">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -2851,25 +2852,25 @@
         <v>2</v>
       </c>
       <c r="G25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H25">
         <v>4</v>
       </c>
       <c r="I25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N25">
         <v>4</v>
@@ -2878,16 +2879,16 @@
         <v>4</v>
       </c>
       <c r="P25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q25">
         <v>2</v>
       </c>
       <c r="R25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T25">
         <v>3</v>
@@ -2896,19 +2897,19 @@
         <v>2</v>
       </c>
       <c r="V25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="W25">
         <v>2</v>
       </c>
       <c r="X25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Y25">
         <v>0</v>
       </c>
       <c r="Z25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA25">
         <v>4</v>
@@ -2920,7 +2921,7 @@
         <v>2</v>
       </c>
       <c r="AD25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE25">
         <v>2</v>
@@ -2928,7 +2929,7 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -2946,25 +2947,25 @@
         <v>2</v>
       </c>
       <c r="G26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H26">
         <v>4</v>
       </c>
       <c r="I26">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K26">
         <v>3</v>
       </c>
       <c r="L26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N26">
         <v>4</v>
@@ -2973,40 +2974,40 @@
         <v>4</v>
       </c>
       <c r="P26">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q26">
         <v>2</v>
       </c>
       <c r="R26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S26">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U26">
         <v>2</v>
       </c>
       <c r="V26">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="W26">
         <v>2</v>
       </c>
       <c r="X26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Y26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z26">
         <v>0</v>
       </c>
       <c r="AA26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB26">
         <v>4</v>
@@ -3023,7 +3024,7 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -3041,43 +3042,43 @@
         <v>2</v>
       </c>
       <c r="G27">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I27">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K27">
         <v>4</v>
       </c>
       <c r="L27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M27">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O27">
         <v>4</v>
       </c>
       <c r="P27">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q27">
         <v>2</v>
       </c>
       <c r="R27">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T27">
         <v>4</v>
@@ -3086,31 +3087,31 @@
         <v>2</v>
       </c>
       <c r="V27">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="W27">
         <v>2</v>
       </c>
       <c r="X27">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Y27">
         <v>4</v>
       </c>
       <c r="Z27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AA27">
         <v>0</v>
       </c>
       <c r="AB27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC27">
         <v>2</v>
       </c>
       <c r="AD27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE27">
         <v>2</v>
@@ -3118,7 +3119,7 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -3136,43 +3137,43 @@
         <v>2</v>
       </c>
       <c r="G28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H28">
         <v>4</v>
       </c>
       <c r="I28">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K28">
         <v>3</v>
       </c>
       <c r="L28">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P28">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q28">
         <v>2</v>
       </c>
       <c r="R28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S28">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T28">
         <v>4</v>
@@ -3181,13 +3182,13 @@
         <v>2</v>
       </c>
       <c r="V28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W28">
         <v>2</v>
       </c>
       <c r="X28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Y28">
         <v>4</v>
@@ -3196,7 +3197,7 @@
         <v>4</v>
       </c>
       <c r="AA28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB28">
         <v>0</v>
@@ -3205,7 +3206,7 @@
         <v>2</v>
       </c>
       <c r="AD28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE28">
         <v>2</v>
@@ -3231,25 +3232,25 @@
         <v>4</v>
       </c>
       <c r="G29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H29">
         <v>2</v>
       </c>
       <c r="I29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K29">
         <v>2</v>
       </c>
       <c r="L29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N29">
         <v>2</v>
@@ -3258,16 +3259,16 @@
         <v>2</v>
       </c>
       <c r="P29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q29">
         <v>3</v>
       </c>
       <c r="R29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T29">
         <v>2</v>
@@ -3276,13 +3277,13 @@
         <v>4</v>
       </c>
       <c r="V29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W29">
         <v>4</v>
       </c>
       <c r="X29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Y29">
         <v>2</v>
@@ -3326,43 +3327,43 @@
         <v>2</v>
       </c>
       <c r="G30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H30">
         <v>4</v>
       </c>
       <c r="I30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K30">
         <v>4</v>
       </c>
       <c r="L30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N30">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q30">
         <v>2</v>
       </c>
       <c r="R30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T30">
         <v>3</v>
@@ -3371,25 +3372,25 @@
         <v>2</v>
       </c>
       <c r="V30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="W30">
         <v>2</v>
       </c>
       <c r="X30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Z30">
         <v>4</v>
       </c>
       <c r="AA30">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC30">
         <v>2</v>
@@ -3421,25 +3422,25 @@
         <v>4</v>
       </c>
       <c r="G31">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H31">
         <v>2</v>
       </c>
       <c r="I31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K31">
         <v>2</v>
       </c>
       <c r="L31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M31">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N31">
         <v>2</v>
@@ -3448,16 +3449,16 @@
         <v>2</v>
       </c>
       <c r="P31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T31">
         <v>2</v>
@@ -3466,13 +3467,13 @@
         <v>4</v>
       </c>
       <c r="V31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W31">
         <v>4</v>
       </c>
       <c r="X31">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Y31">
         <v>2</v>

</xml_diff>